<commit_message>
Adding NASA data products
</commit_message>
<xml_diff>
--- a/Data-Sources/NASA EarthData LANCE and VIIRS Data products.xlsx
+++ b/Data-Sources/NASA EarthData LANCE and VIIRS Data products.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abusharaf/Me.Projects/CallForCode/self-development/Data Sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abusharaf/Me.Projects/CallForCode/teamcodered/documents/Data-Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15FAEAE-171C-B54C-B501-7EA883805B76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0CAB68-11CA-1442-BC85-B1C1CD165CA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Products" sheetId="1" r:id="rId1"/>
@@ -1363,20 +1363,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1392,13 +1378,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1410,16 +1413,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1741,7 +1741,7 @@
   </sheetPr>
   <dimension ref="A2:K126"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -1751,40 +1751,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="12"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
@@ -1890,13 +1890,13 @@
       <c r="D7" s="3">
         <v>107.35</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="14">
+      <c r="E7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="21">
         <v>1</v>
       </c>
       <c r="H7" s="4">
@@ -1923,9 +1923,9 @@
       <c r="D8" s="3">
         <v>8.2799999999999994</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="4">
         <v>0.45</v>
       </c>
@@ -1949,13 +1949,13 @@
       <c r="D9" s="3">
         <v>31.09</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="F9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="21">
         <v>2</v>
       </c>
       <c r="H9" s="4">
@@ -1981,9 +1981,9 @@
       <c r="D10" s="3">
         <v>20.54</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="4">
         <v>0.68</v>
       </c>
@@ -2007,9 +2007,9 @@
       <c r="D11" s="3">
         <v>21.95</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="4">
         <v>0.68</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="14">
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="21">
         <v>3</v>
       </c>
       <c r="H13" s="4">
@@ -2101,8 +2101,8 @@
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="3">
         <v>0.6</v>
       </c>
@@ -2129,10 +2129,10 @@
       <c r="E15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="14">
+      <c r="F15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="21">
         <v>4</v>
       </c>
       <c r="H15" s="4">
@@ -2161,8 +2161,8 @@
       <c r="E16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="4">
         <v>0.82</v>
       </c>
@@ -2190,8 +2190,8 @@
       <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="4">
         <v>0.64</v>
       </c>
@@ -2254,11 +2254,11 @@
       <c r="G19" s="3">
         <v>122</v>
       </c>
-      <c r="H19" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="H19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="2" t="s">
         <v>64</v>
       </c>
@@ -2273,13 +2273,13 @@
       <c r="D20" s="3">
         <v>0.01</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="14">
+      <c r="E20" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="21">
         <v>96</v>
       </c>
       <c r="H20" s="8">
@@ -2305,9 +2305,9 @@
       <c r="D21" s="3">
         <v>0.01</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="4">
         <v>0.5</v>
       </c>
@@ -2331,9 +2331,9 @@
       <c r="D22" s="3">
         <v>0.01</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="3">
         <v>0.5</v>
       </c>
@@ -2366,11 +2366,11 @@
       <c r="G23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="H23" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
       <c r="K23" s="2" t="s">
         <v>75</v>
       </c>
@@ -2417,13 +2417,13 @@
       <c r="D25" s="3">
         <v>107.47</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="14">
+      <c r="E25" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="21">
         <v>1</v>
       </c>
       <c r="H25" s="4">
@@ -2449,9 +2449,9 @@
       <c r="D26" s="3">
         <v>8.2799999999999994</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
       <c r="H26" s="4">
         <v>0.68</v>
       </c>
@@ -2475,13 +2475,13 @@
       <c r="D27" s="3">
         <v>29.53</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="14">
+      <c r="F27" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="21">
         <v>2</v>
       </c>
       <c r="H27" s="4">
@@ -2507,9 +2507,9 @@
       <c r="D28" s="3">
         <v>18.690000000000001</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="4">
         <v>0.82</v>
       </c>
@@ -2533,9 +2533,9 @@
       <c r="D29" s="3">
         <v>22.08</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
       <c r="H29" s="4">
         <v>0.82</v>
       </c>
@@ -2594,10 +2594,10 @@
       <c r="E31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="14">
+      <c r="F31" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="21">
         <v>3</v>
       </c>
       <c r="H31" s="4">
@@ -2626,8 +2626,8 @@
       <c r="E32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
       <c r="H32" s="4">
         <v>0.86</v>
       </c>
@@ -2651,13 +2651,13 @@
       <c r="D33" s="3">
         <v>0.36</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="14">
+      <c r="F33" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="21">
         <v>4</v>
       </c>
       <c r="H33" s="4">
@@ -2683,9 +2683,9 @@
       <c r="D34" s="3">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="4">
         <v>0.99</v>
       </c>
@@ -2712,8 +2712,8 @@
       <c r="E35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="4">
         <v>0.98</v>
       </c>
@@ -2792,40 +2792,40 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="11" t="s">
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
       <c r="H40" s="1" t="s">
         <v>8</v>
       </c>
@@ -2835,7 +2835,7 @@
       <c r="J40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
@@ -2870,40 +2870,40 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H43" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="11" t="s">
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
       <c r="H44" s="1" t="s">
         <v>8</v>
       </c>
@@ -2913,7 +2913,7 @@
       <c r="J44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B45" s="2" t="s">
@@ -3089,20 +3089,20 @@
       <c r="D50" s="3">
         <v>3.2</v>
       </c>
-      <c r="E50" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="14">
+      <c r="E50" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="21">
         <v>12</v>
       </c>
-      <c r="H50" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
+      <c r="H50" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
       <c r="K50" s="2" t="s">
         <v>129</v>
       </c>
@@ -3117,12 +3117,12 @@
       <c r="D51" s="3">
         <v>6.37</v>
       </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
       <c r="K51" s="2" t="s">
         <v>132</v>
       </c>
@@ -3137,12 +3137,12 @@
       <c r="D52" s="3">
         <v>24.54</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
       <c r="K52" s="2" t="s">
         <v>135</v>
       </c>
@@ -3157,20 +3157,20 @@
       <c r="D53" s="3">
         <v>32.909999999999997</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="14">
-        <v>13</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
+      <c r="F53" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="21">
+        <v>13</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
       <c r="K53" s="2" t="s">
         <v>139</v>
       </c>
@@ -3185,12 +3185,12 @@
       <c r="D54" s="3">
         <v>32.43</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
       <c r="K54" s="2" t="s">
         <v>142</v>
       </c>
@@ -3205,14 +3205,14 @@
       <c r="D55" s="3">
         <v>29.02</v>
       </c>
-      <c r="E55" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
+      <c r="E55" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
       <c r="K55" s="2" t="s">
         <v>145</v>
       </c>
@@ -3227,12 +3227,12 @@
       <c r="D56" s="3">
         <v>38.28</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
       <c r="K56" s="2" t="s">
         <v>148</v>
       </c>
@@ -3247,12 +3247,12 @@
       <c r="D57" s="3">
         <v>0.88</v>
       </c>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
       <c r="K57" s="2" t="s">
         <v>151</v>
       </c>
@@ -3267,12 +3267,12 @@
       <c r="D58" s="3">
         <v>4.04</v>
       </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
       <c r="K58" s="2" t="s">
         <v>154</v>
       </c>
@@ -3290,17 +3290,17 @@
       <c r="E59" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="14">
+      <c r="F59" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="21">
         <v>75</v>
       </c>
-      <c r="H59" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
+      <c r="H59" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
       <c r="K59" s="2" t="s">
         <v>157</v>
       </c>
@@ -3318,11 +3318,11 @@
       <c r="E60" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
       <c r="K60" s="2" t="s">
         <v>161</v>
       </c>
@@ -3340,17 +3340,17 @@
       <c r="E61" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="14" t="s">
+      <c r="F61" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
+      <c r="H61" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
       <c r="K61" s="2" t="s">
         <v>166</v>
       </c>
@@ -3368,11 +3368,11 @@
       <c r="E62" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
       <c r="K62" s="2" t="s">
         <v>169</v>
       </c>
@@ -3390,17 +3390,17 @@
       <c r="E63" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="14" t="s">
+      <c r="F63" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="H63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
+      <c r="H63" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
       <c r="K63" s="2" t="s">
         <v>174</v>
       </c>
@@ -3418,11 +3418,11 @@
       <c r="E64" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
       <c r="K64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3601,20 +3601,20 @@
       <c r="D70" s="3">
         <v>3.22</v>
       </c>
-      <c r="E70" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" s="14">
+      <c r="E70" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="21">
         <v>12</v>
       </c>
-      <c r="H70" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
+      <c r="H70" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="19"/>
+      <c r="J70" s="19"/>
       <c r="K70" s="2" t="s">
         <v>190</v>
       </c>
@@ -3629,12 +3629,12 @@
       <c r="D71" s="3">
         <v>6.36</v>
       </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
       <c r="K71" s="2" t="s">
         <v>192</v>
       </c>
@@ -3649,12 +3649,12 @@
       <c r="D72" s="3">
         <v>24.5</v>
       </c>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
       <c r="K72" s="2" t="s">
         <v>194</v>
       </c>
@@ -3669,20 +3669,20 @@
       <c r="D73" s="3">
         <v>30.69</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="E73" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F73" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G73" s="14">
-        <v>13</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
+      <c r="F73" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="21">
+        <v>13</v>
+      </c>
+      <c r="H73" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
       <c r="K73" s="2" t="s">
         <v>196</v>
       </c>
@@ -3697,12 +3697,12 @@
       <c r="D74" s="3">
         <v>31.06</v>
       </c>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
       <c r="K74" s="2" t="s">
         <v>198</v>
       </c>
@@ -3717,14 +3717,14 @@
       <c r="D75" s="3">
         <v>27.46</v>
       </c>
-      <c r="E75" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
+      <c r="E75" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
       <c r="K75" s="2" t="s">
         <v>200</v>
       </c>
@@ -3739,12 +3739,12 @@
       <c r="D76" s="3">
         <v>38.159999999999997</v>
       </c>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="12"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
       <c r="K76" s="2" t="s">
         <v>202</v>
       </c>
@@ -3759,12 +3759,12 @@
       <c r="D77" s="3">
         <v>0.89</v>
       </c>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
       <c r="K77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3779,12 +3779,12 @@
       <c r="D78" s="3">
         <v>4.08</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
       <c r="K78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3802,17 +3802,17 @@
       <c r="E79" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F79" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G79" s="14">
+      <c r="F79" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="21">
         <v>75</v>
       </c>
-      <c r="H79" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
+      <c r="H79" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
       <c r="K79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3830,50 +3830,50 @@
       <c r="E80" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
       <c r="K80" s="2" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="82" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D82" s="11" t="s">
+      <c r="D82" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E82" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F82" s="11" t="s">
+      <c r="F82" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G82" s="11" t="s">
+      <c r="G82" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H82" s="11" t="s">
+      <c r="H82" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
-      <c r="K82" s="11" t="s">
+      <c r="I82" s="19"/>
+      <c r="J82" s="19"/>
+      <c r="K82" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="83" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
       <c r="H83" s="1" t="s">
         <v>8</v>
       </c>
@@ -3883,7 +3883,7 @@
       <c r="J83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K83" s="12"/>
+      <c r="K83" s="19"/>
     </row>
     <row r="84" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B84" s="2" t="s">
@@ -4047,40 +4047,40 @@
       </c>
     </row>
     <row r="92" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="D92" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E92" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="F92" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G92" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H92" s="11" t="s">
+      <c r="H92" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="11" t="s">
+      <c r="I92" s="19"/>
+      <c r="J92" s="19"/>
+      <c r="K92" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="93" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
       <c r="H93" s="1" t="s">
         <v>8</v>
       </c>
@@ -4090,7 +4090,7 @@
       <c r="J93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K93" s="12"/>
+      <c r="K93" s="19"/>
     </row>
     <row r="94" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B94" s="2" t="s">
@@ -4824,40 +4824,40 @@
       </c>
     </row>
     <row r="118" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D118" s="11" t="s">
+      <c r="D118" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E118" s="11" t="s">
+      <c r="E118" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F118" s="11" t="s">
+      <c r="F118" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G118" s="11" t="s">
+      <c r="G118" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H118" s="11" t="s">
+      <c r="H118" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I118" s="12"/>
-      <c r="J118" s="12"/>
-      <c r="K118" s="11" t="s">
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="119" spans="2:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
       <c r="H119" s="1" t="s">
         <v>8</v>
       </c>
@@ -4867,7 +4867,7 @@
       <c r="J119" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K119" s="12"/>
+      <c r="K119" s="19"/>
     </row>
     <row r="120" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B120" s="2" t="s">
@@ -5095,37 +5095,60 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="H118:J118"/>
-    <mergeCell ref="K118:K119"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:J52"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:K93"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="K82:K83"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F73:F78"/>
+    <mergeCell ref="G73:G78"/>
+    <mergeCell ref="H73:J78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:J80"/>
+    <mergeCell ref="H82:J82"/>
     <mergeCell ref="F33:F35"/>
     <mergeCell ref="G33:G35"/>
     <mergeCell ref="H61:J62"/>
@@ -5143,62 +5166,39 @@
     <mergeCell ref="G61:G62"/>
     <mergeCell ref="F63:F64"/>
     <mergeCell ref="G63:G64"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F73:F78"/>
-    <mergeCell ref="G73:G78"/>
-    <mergeCell ref="H73:J78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:J80"/>
-    <mergeCell ref="H82:J82"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:J39"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="K82:K83"/>
-    <mergeCell ref="E70:E72"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:J52"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="H118:J118"/>
+    <mergeCell ref="K118:K119"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:K93"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5569,7 +5569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28568968-42E8-5A4E-81D4-639C2531683F}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -5581,329 +5581,329 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="25"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="25"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A6" s="25"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="26"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A9" s="28"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="29"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A12" s="31"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="24" t="s">
         <v>365</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A14" s="33"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="16" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Adding more smaple sensors data
</commit_message>
<xml_diff>
--- a/Data-Sources/NASA EarthData LANCE and VIIRS Data products.xlsx
+++ b/Data-Sources/NASA EarthData LANCE and VIIRS Data products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abusharaf/Me.Projects/CallForCode/teamcodered/documents/Data-Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0CAB68-11CA-1442-BC85-B1C1CD165CA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8826E77F-0E80-4346-BDCD-1CAF9CCB4CA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1197,7 +1197,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1237,6 +1237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1343,7 +1349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1422,6 +1428,14 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1741,8 +1755,8 @@
   </sheetPr>
   <dimension ref="A2:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2057,16 +2071,16 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6"/>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="36">
         <v>1.71</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="37" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="21" t="s">
@@ -2873,7 +2887,7 @@
       <c r="B43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="34" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="18" t="s">
@@ -2983,16 +2997,16 @@
       <c r="A47" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="36">
         <v>4.91</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="35" t="s">
         <v>117</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -4188,7 +4202,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B97" s="2" t="s">
         <v>245</v>
       </c>
@@ -4220,7 +4234,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B98" s="2" t="s">
         <v>249</v>
       </c>
@@ -4252,7 +4266,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B99" s="2" t="s">
         <v>252</v>
       </c>
@@ -4284,7 +4298,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B100" s="2" t="s">
         <v>255</v>
       </c>
@@ -4316,7 +4330,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B101" s="2" t="s">
         <v>258</v>
       </c>
@@ -4348,7 +4362,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B102" s="2" t="s">
         <v>262</v>
       </c>
@@ -4380,7 +4394,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B103" s="2" t="s">
         <v>265</v>
       </c>
@@ -4412,7 +4426,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="104" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B104" s="2" t="s">
         <v>268</v>
       </c>
@@ -4444,7 +4458,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="105" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B105" s="2" t="s">
         <v>271</v>
       </c>
@@ -4472,7 +4486,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A106" s="5"/>
       <c r="B106" s="2" t="s">
         <v>275</v>
       </c>
@@ -4498,7 +4513,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="107" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B107" s="2" t="s">
         <v>279</v>
       </c>
@@ -4530,7 +4545,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="108" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B108" s="2" t="s">
         <v>282</v>
       </c>
@@ -4562,7 +4577,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="109" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B109" s="2" t="s">
         <v>285</v>
       </c>
@@ -4594,7 +4609,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="110" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B110" s="2" t="s">
         <v>289</v>
       </c>
@@ -4626,7 +4641,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="111" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B111" s="2" t="s">
         <v>292</v>
       </c>
@@ -4658,7 +4673,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="112" spans="2:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B112" s="2" t="s">
         <v>295</v>
       </c>
@@ -5095,75 +5110,22 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="K82:K83"/>
-    <mergeCell ref="E70:E72"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F73:F78"/>
-    <mergeCell ref="G73:G78"/>
-    <mergeCell ref="H73:J78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:J80"/>
-    <mergeCell ref="H82:J82"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="H61:J62"/>
-    <mergeCell ref="H63:J64"/>
-    <mergeCell ref="H70:J72"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F58"/>
-    <mergeCell ref="G53:G58"/>
-    <mergeCell ref="H53:J58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:J60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H118:J118"/>
+    <mergeCell ref="K118:K119"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:K93"/>
     <mergeCell ref="F63:F64"/>
     <mergeCell ref="G63:G64"/>
     <mergeCell ref="G39:G40"/>
@@ -5183,22 +5145,75 @@
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="G43:G44"/>
     <mergeCell ref="E50:E52"/>
-    <mergeCell ref="H118:J118"/>
-    <mergeCell ref="K118:K119"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:K93"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F73:F78"/>
+    <mergeCell ref="G73:G78"/>
+    <mergeCell ref="H73:J78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:J80"/>
+    <mergeCell ref="H82:J82"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="K82:K83"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="H61:J62"/>
+    <mergeCell ref="H63:J64"/>
+    <mergeCell ref="H70:J72"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F58"/>
+    <mergeCell ref="G53:G58"/>
+    <mergeCell ref="H53:J58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:J60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>